<commit_message>
update data on dashboard
</commit_message>
<xml_diff>
--- a/document/Q&A.xlsx
+++ b/document/Q&A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Tình trạng câu hỏi
 (Open, Closed)</t>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Q&amp;A</t>
+  </si>
+  <si>
+    <t>Câu truy vấn lấy quý hiện tại</t>
+  </si>
+  <si>
+    <t>Đào Hoài Phương</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -129,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -144,6 +153,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +458,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,14 +524,24 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6">
+        <v>42959</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>

</xml_diff>